<commit_message>
Standard User name change in Contacts test data files - 6th Mar 2024
</commit_message>
<xml_diff>
--- a/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
+++ b/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD938CCA-2CD6-4BD6-BD66-D8A3EA2F655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22530" windowHeight="5280" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -71,9 +72,6 @@
     <t>ActivityCompany</t>
   </si>
   <si>
-    <t>Drew Koecher</t>
-  </si>
-  <si>
     <t>Quick Link</t>
   </si>
   <si>
@@ -114,12 +112,15 @@
   </si>
   <si>
     <t>Accounts (Primary Billing Contact)</t>
+  </si>
+  <si>
+    <t>Ayati Arvind</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,25 +441,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -500,7 +501,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -508,86 +509,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -596,24 +597,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -625,28 +626,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contacts Migration: LV_T1047_T1100_T1941_T1945_T2146_T2145_Contact_CreateNewContactRecordTypeExternalContact - 19 July 2024
</commit_message>
<xml_diff>
--- a/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
+++ b/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD938CCA-2CD6-4BD6-BD66-D8A3EA2F655E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1FD9A5-2DFE-4380-9B01-19D771323CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>CompanyName</t>
   </si>
@@ -39,15 +39,9 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>ContactTypesValue</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
-    <t>StdUser</t>
-  </si>
-  <si>
     <t>External Contact</t>
   </si>
   <si>
@@ -114,7 +108,22 @@
     <t>Accounts (Primary Billing Contact)</t>
   </si>
   <si>
-    <t>Ayati Arvind</t>
+    <t>Amanda Donovan</t>
+  </si>
+  <si>
+    <t>CF Financial User</t>
+  </si>
+  <si>
+    <t>Contact Full Name</t>
+  </si>
+  <si>
+    <t>Test ExternalContact</t>
+  </si>
+  <si>
+    <t>AdminUser</t>
+  </si>
+  <si>
+    <t>Indrajeet Singh</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,12 +463,11 @@
     <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,39 +477,39 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
+      <c r="F2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -523,72 +531,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -611,12 +619,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +638,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,13 +649,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contacts Migration - 19 July 2024
</commit_message>
<xml_diff>
--- a/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
+++ b/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1FD9A5-2DFE-4380-9B01-19D771323CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190B5E8F-CD88-41C7-93C5-4ECC5D5B4CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>CompanyName</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Quick Link</t>
   </si>
   <si>
-    <t>Activities</t>
-  </si>
-  <si>
     <t>HL Relationships</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Opportunity Contacts</t>
   </si>
   <si>
-    <t>Engagement Contacts</t>
-  </si>
-  <si>
     <t>Engagements Shown</t>
   </si>
   <si>
@@ -102,12 +96,6 @@
     <t>Contact History</t>
   </si>
   <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>Accounts (Primary Billing Contact)</t>
-  </si>
-  <si>
     <t>Amanda Donovan</t>
   </si>
   <si>
@@ -124,6 +112,24 @@
   </si>
   <si>
     <t>Indrajeet Singh</t>
+  </si>
+  <si>
+    <t>Engagement Contacts (Contact)</t>
+  </si>
+  <si>
+    <t>Related Companies</t>
+  </si>
+  <si>
+    <t>Memberships</t>
+  </si>
+  <si>
+    <t>Contact Email History</t>
+  </si>
+  <si>
+    <t>Development Leads</t>
+  </si>
+  <si>
+    <t>Files</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -504,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,52 +557,62 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -649,18 +665,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LV_T1047_T1100_T1941_T1945_T2146_T2145_Contact_CreateNewContactRecordTypeExternalContact - 30 July 2024
</commit_message>
<xml_diff>
--- a/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
+++ b/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190B5E8F-CD88-41C7-93C5-4ECC5D5B4CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C85EB-9760-49B2-8440-22F4C07DB67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
-    <sheet name="QuickLink" sheetId="4" r:id="rId2"/>
+    <sheet name="QuickLinks" sheetId="4" r:id="rId2"/>
     <sheet name="ContactTypes" sheetId="3" r:id="rId3"/>
     <sheet name="Users" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -66,9 +66,6 @@
     <t>ActivityCompany</t>
   </si>
   <si>
-    <t>Quick Link</t>
-  </si>
-  <si>
     <t>HL Relationships</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Files</t>
+  </si>
+  <si>
+    <t>Quick Links</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -526,9 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -537,82 +535,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -665,18 +663,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LV_T1048_T1942_T1943_T1944_T1945_T1946_T1951_T1954_T1955_T1957_T1958_Contact_CreateNewContactRecordTypeHoulihanEmployee - 30 July 2024
</commit_message>
<xml_diff>
--- a/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
+++ b/TestData/T1047_Contact_CreateNewContactRecordTypeExternalContact.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C85EB-9760-49B2-8440-22F4C07DB67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DA16E9-3A59-4F3E-B1A2-43663BD5D763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -651,13 +651,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>